<commit_message>
get excel from mohammad and reza and fix CL max
</commit_message>
<xml_diff>
--- a/Matching Diagram/Landing.xlsx
+++ b/Matching Diagram/Landing.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B80DB18-7319-41DF-B30D-16C9BFD0F25D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{978D7904-3495-4776-B5F8-DE0E64F7A806}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -247,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -283,12 +283,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,6 +328,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C7:K60"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:AB20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,10 +646,10 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
@@ -681,8 +695,8 @@
         <v>47</v>
       </c>
       <c r="E12" s="6">
-        <f>4000/0.6</f>
-        <v>6666.666666666667</v>
+        <f>4000*1.4</f>
+        <v>5600</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>18</v>
@@ -696,8 +710,8 @@
         <v>47</v>
       </c>
       <c r="E13" s="8">
-        <f>6000/0.6</f>
-        <v>10000</v>
+        <f>6000*1.4</f>
+        <v>8400</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>18</v>
@@ -712,7 +726,7 @@
       </c>
       <c r="E14" s="7">
         <f>SQRT(E12/0.3)</f>
-        <v>149.07119849998597</v>
+        <v>136.62601021279465</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>3</v>
@@ -727,7 +741,7 @@
       </c>
       <c r="E15" s="9">
         <f>SQRT(E13/0.3)</f>
-        <v>182.57418583505537</v>
+        <v>167.33200530681512</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>3</v>
@@ -742,7 +756,7 @@
       </c>
       <c r="E16" s="6">
         <f>E14/1.3</f>
-        <v>114.6701526922969</v>
+        <v>105.09693093291897</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -755,7 +769,7 @@
       </c>
       <c r="E17" s="8">
         <f>E15/1.3</f>
-        <v>140.44168141158104</v>
+        <v>128.71692715908856</v>
       </c>
       <c r="K17">
         <f>1/K18</f>
@@ -770,7 +784,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="2">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="K18">
         <f>48.5/42.549</f>
@@ -785,7 +799,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="2">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>21</v>
@@ -839,7 +853,7 @@
       </c>
       <c r="E25" s="6">
         <f>E16^2*ro*E18*1.688^2/2</f>
-        <v>129.13092127810651</v>
+        <v>115.70130546518347</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>40</v>
@@ -849,12 +863,12 @@
       </c>
       <c r="I25" s="11">
         <f>E16^2*E22*E18*1.688^2/2</f>
-        <v>111.11317598422087</v>
-      </c>
-      <c r="J25" s="21" t="s">
+        <v>99.557405681861937</v>
+      </c>
+      <c r="J25" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="21"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D26" s="2" t="s">
@@ -862,14 +876,14 @@
       </c>
       <c r="E26" s="4">
         <f>E25/E9</f>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I26" s="12">
         <f>I25/E9</f>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
@@ -884,7 +898,7 @@
       </c>
       <c r="E28" s="6">
         <f>E16^2*ro*CL_max*1.688^2/2</f>
-        <v>120.52219319289939</v>
+        <v>108.46997387360949</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>41</v>
@@ -894,12 +908,12 @@
       </c>
       <c r="I28" s="11">
         <f>E16^2*E22*CL_max*1.688^2/2</f>
-        <v>103.70563091860613</v>
-      </c>
-      <c r="J28" s="21" t="s">
+        <v>93.335067826745558</v>
+      </c>
+      <c r="J28" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="21"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D29" s="2" t="s">
@@ -907,14 +921,14 @@
       </c>
       <c r="E29" s="4">
         <f>E28/E9</f>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I29" s="12">
         <f>I28/E9</f>
-        <v>118.21013653793032</v>
+        <v>106.38912288413734</v>
       </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
@@ -929,7 +943,7 @@
       </c>
       <c r="E31" s="6">
         <f>E16^2*ro*E20*1.688^2/2</f>
-        <v>116.21782915029586</v>
+        <v>97.622976486248547</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>42</v>
@@ -939,12 +953,12 @@
       </c>
       <c r="I31" s="11">
         <f>E16^2*E22*E20*1.688^2/2</f>
-        <v>100.00185838579878</v>
-      </c>
-      <c r="J31" s="21" t="s">
+        <v>84.001561044071011</v>
+      </c>
+      <c r="J31" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K31" s="21"/>
+      <c r="K31" s="22"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
@@ -952,14 +966,14 @@
       </c>
       <c r="E32" s="4">
         <f>E31/E9</f>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I32" s="12">
         <f>I31/E9</f>
-        <v>113.98834594728997</v>
+        <v>95.750210595723615</v>
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
@@ -974,7 +988,7 @@
       </c>
       <c r="E34" s="8">
         <f>V_SL^2*ro*E18*1.688^2/2</f>
-        <v>193.69638191715978</v>
+        <v>173.55195819777518</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>43</v>
@@ -984,12 +998,12 @@
       </c>
       <c r="I34" s="14">
         <f>V_SL^2*E18*E22*1.688^2/2</f>
-        <v>166.66976397633132</v>
-      </c>
-      <c r="J34" s="21" t="s">
+        <v>149.3361085227929</v>
+      </c>
+      <c r="J34" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="21"/>
+      <c r="K34" s="22"/>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
@@ -997,14 +1011,14 @@
       </c>
       <c r="E35" s="4">
         <f>E34/E10</f>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I35" s="12">
         <f>I34/E10</f>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
@@ -1019,7 +1033,7 @@
       </c>
       <c r="E37" s="8">
         <f>V_SL^2*ro*CL_max*1.688^2/2</f>
-        <v>180.78328978934908</v>
+        <v>162.70496081041424</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>44</v>
@@ -1029,12 +1043,12 @@
       </c>
       <c r="I37" s="14">
         <f>V_SL^2*E22*CL_max*1.688^2/2</f>
-        <v>155.55844637790923</v>
-      </c>
-      <c r="J37" s="21" t="s">
+        <v>140.00260174011834</v>
+      </c>
+      <c r="J37" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K37" s="21"/>
+      <c r="K37" s="22"/>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
@@ -1043,7 +1057,7 @@
       </c>
       <c r="E38" s="4">
         <f>E37/E10</f>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
@@ -1051,7 +1065,7 @@
       </c>
       <c r="I38" s="12">
         <f>I37/E10</f>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
@@ -1066,7 +1080,7 @@
       </c>
       <c r="E40" s="8">
         <f>V_SL^2*ro*E20*1.688^2/2</f>
-        <v>174.32674372544378</v>
+        <v>146.43446472937282</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>45</v>
@@ -1076,12 +1090,12 @@
       </c>
       <c r="I40" s="14">
         <f>V_SL^2*E22*E20*1.688^2/2</f>
-        <v>150.00278757869819</v>
-      </c>
-      <c r="J40" s="21" t="s">
+        <v>126.00234156610651</v>
+      </c>
+      <c r="J40" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K40" s="21"/>
+      <c r="K40" s="22"/>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
@@ -1089,26 +1103,26 @@
       </c>
       <c r="E41" s="4">
         <f>E40/E10</f>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I41" s="12">
         <f>I40/E10</f>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="2"/>
@@ -1275,11 +1289,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AA471B-9061-4721-96F4-C2B8E98F9333}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,7 +1302,13 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1310,7 +1330,7 @@
       <c r="F1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="20" t="s">
         <v>33</v>
       </c>
       <c r="H1" s="18"/>
@@ -1342,54 +1362,55 @@
       </c>
       <c r="B2" s="2">
         <f>Sheet1!E26</f>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C2" s="2">
         <f>Sheet1!E29</f>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D2" s="2">
         <f>Sheet1!E32</f>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E2" s="2">
         <f>Sheet1!I26</f>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F2" s="2">
         <f>Sheet1!I29</f>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G2" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G2" s="22">
         <f>Sheet1!I32</f>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H2" s="22"/>
       <c r="I2" s="15">
         <v>0</v>
       </c>
       <c r="J2" s="15">
         <f>Sheet1!E35</f>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K2" s="15">
         <f>Sheet1!E38</f>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L2" s="15">
         <f>Sheet1!E41</f>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M2" s="15">
         <f>Sheet1!I35</f>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N2" s="15">
         <f>Sheet1!I38</f>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O2" s="15">
         <f>Sheet1!I41</f>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1398,54 +1419,55 @@
       </c>
       <c r="B3" s="2">
         <f t="shared" ref="B3:B20" si="0">B2</f>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C20" si="1">C2</f>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D20" si="2">D2</f>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E20" si="3">E2</f>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F20" si="4">F2</f>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G3" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G3" s="22">
         <f t="shared" ref="G3:G20" si="5">G2</f>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H3" s="22"/>
       <c r="I3" s="15">
         <v>0.05</v>
       </c>
       <c r="J3" s="15">
         <f t="shared" ref="J3:J20" si="6">J2</f>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K3" s="15">
         <f t="shared" ref="K3:K20" si="7">K2</f>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L3" s="15">
         <f t="shared" ref="L3:L20" si="8">L2</f>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M3" s="15">
         <f t="shared" ref="M3:M20" si="9">M2</f>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N3" s="15">
         <f t="shared" ref="N3:N20" si="10">N2</f>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O3" s="15">
         <f t="shared" ref="O3:O20" si="11">O2</f>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1454,54 +1476,55 @@
       </c>
       <c r="B4" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G4" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G4" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H4" s="22"/>
       <c r="I4" s="15">
         <v>0.1</v>
       </c>
       <c r="J4" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K4" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L4" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M4" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N4" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O4" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1510,54 +1533,55 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G5" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G5" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H5" s="22"/>
       <c r="I5" s="15">
         <v>0.15</v>
       </c>
       <c r="J5" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K5" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L5" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M5" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N5" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O5" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1566,54 +1590,55 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G6" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G6" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H6" s="22"/>
       <c r="I6" s="15">
         <v>0.2</v>
       </c>
       <c r="J6" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K6" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L6" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M6" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N6" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O6" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1622,54 +1647,55 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G7" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G7" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H7" s="22"/>
       <c r="I7" s="15">
         <v>0.25</v>
       </c>
       <c r="J7" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K7" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L7" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M7" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N7" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O7" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1678,54 +1704,55 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G8" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G8" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H8" s="22"/>
       <c r="I8" s="15">
         <v>0.3</v>
       </c>
       <c r="J8" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K8" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L8" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M8" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N8" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O8" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1734,54 +1761,55 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G9" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G9" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H9" s="22"/>
       <c r="I9" s="15">
         <v>0.35</v>
       </c>
       <c r="J9" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K9" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L9" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M9" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N9" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O9" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1790,54 +1818,55 @@
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G10" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G10" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H10" s="22"/>
       <c r="I10" s="15">
         <v>0.4</v>
       </c>
       <c r="J10" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K10" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L10" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M10" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N10" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O10" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1846,54 +1875,55 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G11" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G11" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H11" s="22"/>
       <c r="I11" s="15">
         <v>0.45</v>
       </c>
       <c r="J11" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K11" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L11" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M11" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N11" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O11" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1902,54 +1932,55 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G12" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G12" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H12" s="22"/>
       <c r="I12" s="15">
         <v>0.5</v>
       </c>
       <c r="J12" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K12" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L12" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M12" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N12" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O12" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1958,54 +1989,55 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G13" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G13" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H13" s="22"/>
       <c r="I13" s="15">
         <v>0.55000000000000004</v>
       </c>
       <c r="J13" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K13" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L13" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M13" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N13" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O13" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2014,54 +2046,55 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G14" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G14" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H14" s="22"/>
       <c r="I14" s="15">
         <v>0.6</v>
       </c>
       <c r="J14" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K14" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L14" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M14" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N14" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O14" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2070,54 +2103,55 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G15" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G15" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H15" s="22"/>
       <c r="I15" s="15">
         <v>0.65</v>
       </c>
       <c r="J15" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K15" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L15" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M15" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N15" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O15" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2126,54 +2160,55 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G16" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G16" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H16" s="22"/>
       <c r="I16" s="15">
         <v>0.7</v>
       </c>
       <c r="J16" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K16" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L16" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M16" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N16" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O16" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2182,54 +2217,55 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G17" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G17" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H17" s="22"/>
       <c r="I17" s="15">
         <v>0.75</v>
       </c>
       <c r="J17" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K17" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L17" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M17" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N17" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O17" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2238,54 +2274,55 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G18" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G18" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H18" s="22"/>
       <c r="I18" s="15">
         <v>0.8</v>
       </c>
       <c r="J18" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K18" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L18" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M18" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N18" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O18" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2294,54 +2331,55 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G19" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G19" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H19" s="22"/>
       <c r="I19" s="15">
         <v>0.85</v>
       </c>
       <c r="J19" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K19" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M19" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N19" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O19" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2350,57 +2388,79 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" si="0"/>
-        <v>147.19146588611167</v>
+        <v>131.88355343395611</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="1"/>
-        <v>137.3787014937042</v>
+        <v>123.64083134433383</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="2"/>
-        <v>132.47231929750049</v>
+        <v>111.27674820990045</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="3"/>
-        <v>126.65371771921107</v>
+        <v>113.48173107641317</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="4"/>
-        <v>118.21013653793032</v>
-      </c>
-      <c r="G20" s="2">
+        <v>106.38912288413734</v>
+      </c>
+      <c r="G20" s="22">
         <f t="shared" si="5"/>
-        <v>113.98834594728997</v>
-      </c>
+        <v>95.750210595723615</v>
+      </c>
+      <c r="H20" s="22"/>
       <c r="I20" s="15">
         <v>0.9</v>
       </c>
       <c r="J20" s="15">
         <f t="shared" si="6"/>
-        <v>229.9848978831493</v>
+        <v>206.06646850330179</v>
       </c>
       <c r="K20" s="15">
         <f t="shared" si="7"/>
-        <v>214.65257135760595</v>
+        <v>193.18731422184544</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" si="8"/>
-        <v>206.98640809483433</v>
+        <v>173.86858279966089</v>
       </c>
       <c r="M20" s="15">
         <f t="shared" si="9"/>
-        <v>197.89491300203434</v>
+        <v>177.31384204982282</v>
       </c>
       <c r="N20" s="15">
         <f t="shared" si="10"/>
-        <v>184.70191880189873</v>
+        <v>166.23172692170888</v>
       </c>
       <c r="O20" s="15">
         <f t="shared" si="11"/>
-        <v>178.10542170183092</v>
+        <v>149.60855422953802</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>